<commit_message>
updated read and write excel logic
</commit_message>
<xml_diff>
--- a/Test_Suite_Data.xlsx
+++ b/Test_Suite_Data.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E578B8-F9BD-4B43-A210-E7D82E79610E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104709E9-770D-4880-932C-5E9A2CCEA084}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="2775" windowWidth="13605" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="runner" sheetId="1" r:id="rId1"/>
-    <sheet name="data" sheetId="2" r:id="rId2"/>
+    <sheet name="LoginPageTest" sheetId="3" r:id="rId2"/>
+    <sheet name="MyFirstTest" sheetId="4" r:id="rId3"/>
+    <sheet name="data" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
   <si>
     <t>TCID</t>
   </si>
@@ -58,6 +60,18 @@
   </si>
   <si>
     <t>loginPageTitleTest</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>LoginPageTest</t>
+  </si>
+  <si>
+    <t>MyFirstTest</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
@@ -108,7 +122,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -142,12 +156,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -170,6 +197,13 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -509,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,26 +565,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -559,11 +585,139 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC5AED07-E522-4BDF-BA6C-EDACF2962E7E}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1401DA-C691-4F19-B5A7-28C0F4F61E83}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2"/>
+    </row>
+    <row r="3" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3"/>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{2E040103-CE7B-4D37-9E13-EE9F9A65898A}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{934AD996-5D06-464B-B8D6-811173AE1355}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{3C178704-09DD-4CB1-9C24-0C187368F648}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +748,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>5</v>
@@ -605,7 +759,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>5</v>
@@ -633,13 +787,28 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the logic to read data from different class tabs from excel
</commit_message>
<xml_diff>
--- a/Test_Suite_Data.xlsx
+++ b/Test_Suite_Data.xlsx
@@ -3,22 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104709E9-770D-4880-932C-5E9A2CCEA084}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{025BE437-051D-4B49-8420-2D7186C97BD5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="2775" windowWidth="13605" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="2775" windowWidth="13605" windowHeight="5895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="runner" sheetId="1" r:id="rId1"/>
     <sheet name="LoginPageTest" sheetId="3" r:id="rId2"/>
     <sheet name="MyFirstTest" sheetId="4" r:id="rId3"/>
-    <sheet name="data" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>TCID</t>
   </si>
@@ -122,7 +121,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -153,17 +152,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -174,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -190,17 +178,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -545,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -564,7 +549,7 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -589,7 +574,7 @@
   <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -597,8 +582,8 @@
     <col min="1" max="1" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:1" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -621,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F1401DA-C691-4F19-B5A7-28C0F4F61E83}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -632,8 +617,8 @@
     <col min="3" max="3" width="8.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
     </row>
@@ -653,10 +638,10 @@
       <c r="A3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="D3"/>
@@ -673,8 +658,8 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
     </row>
@@ -710,113 +695,4 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="19.85546875" style="3" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="71.5703125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="26" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="55" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="16384" width="9.140625" style="3" collapsed="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="7"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
provided environment specific config files
</commit_message>
<xml_diff>
--- a/Test_Suite_Data.xlsx
+++ b/Test_Suite_Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20730"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{392E3455-6751-4ECB-91CC-726E4DF7AC39}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB5046DE-8E3F-4141-9423-9406A1698C5A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="2775" windowWidth="13605" windowHeight="5895" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,7 +550,7 @@
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>